<commit_message>
Now working, label system is well
still need to update excel by the team
</commit_message>
<xml_diff>
--- a/tag_contacts.xlsx
+++ b/tag_contacts.xlsx
@@ -5,24 +5,37 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gilad.barak/Documents/צבאי/ש7/XOAssistant/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gilad.barak/Documents/צבאי/ש7/XOAssistant/Xo-Assistance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A485308E-8D39-A24C-AD25-3E0D02B515F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86548EB5-30F0-9D42-809F-66F6E16B939F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14360" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contacts_master" sheetId="1" r:id="rId1"/>
     <sheet name="tag_membership" sheetId="2" r:id="rId2"/>
     <sheet name="tag_meta" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
   <si>
     <t>id</t>
   </si>
@@ -36,24 +49,12 @@
     <t>phone</t>
   </si>
   <si>
-    <t>Lt. Dan Example</t>
-  </si>
-  <si>
-    <t>OPS Officer</t>
-  </si>
-  <si>
     <t>ops1@example.mil</t>
   </si>
   <si>
-    <t>+972-50-000-0001</t>
-  </si>
-  <si>
     <t>Ens. Lee Example</t>
   </si>
   <si>
-    <t>Watch</t>
-  </si>
-  <si>
     <t>lee@example.mil</t>
   </si>
   <si>
@@ -63,9 +64,6 @@
     <t>Lt. Noa Example</t>
   </si>
   <si>
-    <t>Navigator</t>
-  </si>
-  <si>
     <t>noa@example.mil</t>
   </si>
   <si>
@@ -75,9 +73,6 @@
     <t>CPO Amir Example</t>
   </si>
   <si>
-    <t>Engineering Chief</t>
-  </si>
-  <si>
     <t>amir@example.mil</t>
   </si>
   <si>
@@ -87,30 +82,6 @@
     <t>contact_email</t>
   </si>
   <si>
-    <t>Technical</t>
-  </si>
-  <si>
-    <t>OPS</t>
-  </si>
-  <si>
-    <t>GNK</t>
-  </si>
-  <si>
-    <t>Command</t>
-  </si>
-  <si>
-    <t>Sonar</t>
-  </si>
-  <si>
-    <t>Weaponry</t>
-  </si>
-  <si>
-    <t>Co</t>
-  </si>
-  <si>
-    <t>Xo</t>
-  </si>
-  <si>
     <t>color_name</t>
   </si>
   <si>
@@ -165,20 +136,59 @@
     <t>2</t>
   </si>
   <si>
-    <t>Team</t>
-  </si>
-  <si>
     <t>Lavender</t>
   </si>
   <si>
     <t>label</t>
+  </si>
+  <si>
+    <t>טכנית</t>
+  </si>
+  <si>
+    <t>גנ״ק</t>
+  </si>
+  <si>
+    <t>פיקוד</t>
+  </si>
+  <si>
+    <t>סונאר</t>
+  </si>
+  <si>
+    <t>נשק</t>
+  </si>
+  <si>
+    <t>סגן</t>
+  </si>
+  <si>
+    <t>מבצעים</t>
+  </si>
+  <si>
+    <t>מפקד</t>
+  </si>
+  <si>
+    <t>צוות</t>
+  </si>
+  <si>
+    <t>Alon Berko</t>
+  </si>
+  <si>
+    <t>ops2@example.com</t>
+  </si>
+  <si>
+    <t>Gilad Brarak</t>
+  </si>
+  <si>
+    <t>giladondon@gmail.com</t>
+  </si>
+  <si>
+    <t>+972-54-450-4730</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +201,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -225,17 +243,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -536,13 +557,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -552,7 +578,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -566,16 +592,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
+        <v>40</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -583,16 +609,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -600,16 +626,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -617,19 +643,40 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D6" r:id="rId1" xr:uid="{46F68578-013B-FB46-9DFC-9EB9CA004F61}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{5739C88A-35D5-1D48-B21B-E64FA1F47C2A}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -639,97 +686,97 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -741,7 +788,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -751,109 +800,109 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
         <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
add emojis to color file
</commit_message>
<xml_diff>
--- a/tag_contacts.xlsx
+++ b/tag_contacts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gilad.barak/Documents/צבאי/ש7/XOAssistant/Xo-Assistance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86548EB5-30F0-9D42-809F-66F6E16B939F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AAC4D0D-4649-B044-9496-4DBCA12A8561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14360" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contacts_master" sheetId="1" r:id="rId1"/>
@@ -151,9 +151,6 @@
     <t>פיקוד</t>
   </si>
   <si>
-    <t>סונאר</t>
-  </si>
-  <si>
     <t>נשק</t>
   </si>
   <si>
@@ -182,6 +179,9 @@
   </si>
   <si>
     <t>+972-54-450-4730</t>
+  </si>
+  <si>
+    <t>סונר</t>
   </si>
 </sst>
 </file>
@@ -559,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -592,16 +592,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -646,7 +646,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -660,13 +660,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="C6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
@@ -686,7 +686,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -733,7 +733,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -741,7 +741,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -757,7 +757,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
@@ -765,7 +765,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -788,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -822,7 +822,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -855,7 +855,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
@@ -866,7 +866,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
         <v>27</v>
@@ -877,7 +877,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
         <v>29</v>
@@ -888,7 +888,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
         <v>31</v>
@@ -899,7 +899,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
         <v>33</v>

</xml_diff>